<commit_message>
changed website name for the project
</commit_message>
<xml_diff>
--- a/Project_Notebook.xlsx
+++ b/Project_Notebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keundong\Documents\UiPath\LoginProcess_Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C491AEB4-2161-49E7-9821-B18A36432BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB37101A-1653-4B15-96A7-C3DBD8E2FA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="2565" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="6840" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -62,6 +62,7 @@
     <definedName name="Trimmed">Text!$B$5</definedName>
     <definedName name="TwoDecimals">Number!$B$7</definedName>
     <definedName name="UpperCase">Text!$B$7</definedName>
+    <definedName name="website">Scratchpad!$B$1</definedName>
     <definedName name="YYYYMMDD">Date!$B$10</definedName>
     <definedName name="비즈메카">Scratchpad!$B$1</definedName>
   </definedNames>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -348,9 +349,6 @@
   </si>
   <si>
     <t>website</t>
-  </si>
-  <si>
-    <t>https://ezsso.bizmeka.com/sso/ssoLogin.do</t>
   </si>
   <si>
     <t>C:\Users\keundong\Documents\PersonalData.xlsx</t>
@@ -1476,8 +1474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95188A8B-20B9-44C0-8B2D-2363D0E3925F}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,9 +1487,6 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>87</v>
-      </c>
-      <c r="B1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1551,7 +1546,7 @@
       </c>
       <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>45103</v>
+        <v>45270</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1571,7 @@
       </c>
       <c r="B8" s="28" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
-        <v>2023-07-03</v>
+        <v>2023-12-17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,7 +1580,7 @@
       </c>
       <c r="B9" s="28" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
-        <v>2023-07-05</v>
+        <v>2023-12-19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1594,7 +1589,7 @@
       </c>
       <c r="B10" s="29" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20230626</v>
+        <v>20231210</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1603,7 +1598,7 @@
       </c>
       <c r="B12" s="28" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>2023-06-26</v>
+        <v>2023-12-10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1612,15 +1607,15 @@
       </c>
       <c r="B13" s="28" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
-        <v>2023-06-19</v>
+        <v>2023-11-27</v>
       </c>
       <c r="C13" s="28" t="str">
         <f ca="1">TEXT(LastWeekMonday+4, preferred_date_format)</f>
-        <v>2023-06-23</v>
+        <v>2023-12-01</v>
       </c>
       <c r="D13" s="30" t="str">
         <f ca="1">TEXT(LastWeekFriday+2, preferred_date_format)</f>
-        <v>2023-06-25</v>
+        <v>2023-12-03</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1629,11 +1624,11 @@
       </c>
       <c r="B14" s="28" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1), preferred_date_format)</f>
-        <v>2023-05-01</v>
+        <v>2023-11-01</v>
       </c>
       <c r="C14" s="28" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), 0), preferred_date_format)</f>
-        <v>2023-05-31</v>
+        <v>2023-11-30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1642,11 +1637,11 @@
       </c>
       <c r="B15" s="28" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1), preferred_date_format)</f>
-        <v>2023-06-01</v>
+        <v>2023-12-01</v>
       </c>
       <c r="C15" s="28" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1), preferred_date_format)</f>
-        <v>2023-06-30</v>
+        <v>2023-12-29</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2189,7 +2184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B15AA95-D2AA-4AD6-8E83-DBFAD20B8498}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2239,7 +2234,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>